<commit_message>
Modify incorrect sport facility file
</commit_message>
<xml_diff>
--- a/data/dohee/2006-2021_종합체육시설 수.xlsx
+++ b/data/dohee/2006-2021_종합체육시설 수.xlsx
@@ -534,52 +534,52 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>581</v>
+        <v>270</v>
       </c>
       <c r="C2">
-        <v>39787</v>
+        <v>318</v>
       </c>
       <c r="D2">
-        <v>823</v>
+        <v>359</v>
       </c>
       <c r="E2">
-        <v>982</v>
+        <v>460</v>
       </c>
       <c r="F2">
-        <v>1019</v>
+        <v>484</v>
       </c>
       <c r="G2">
-        <v>1074</v>
+        <v>518</v>
       </c>
       <c r="H2">
-        <v>1142</v>
+        <v>559</v>
       </c>
       <c r="I2">
-        <v>1182</v>
+        <v>597</v>
       </c>
       <c r="J2">
-        <v>1267</v>
+        <v>670</v>
       </c>
       <c r="K2">
-        <v>1290</v>
+        <v>689</v>
       </c>
       <c r="L2">
-        <v>1326</v>
+        <v>735</v>
       </c>
       <c r="M2">
-        <v>1367</v>
+        <v>778</v>
       </c>
       <c r="N2">
-        <v>1418</v>
+        <v>991</v>
       </c>
       <c r="O2">
-        <v>1435</v>
+        <v>1015</v>
       </c>
       <c r="P2">
-        <v>1457</v>
+        <v>1046</v>
       </c>
       <c r="Q2">
-        <v>1496</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -587,40 +587,40 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
         <v>35</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <v>36</v>
+      </c>
+      <c r="H3">
         <v>40</v>
       </c>
-      <c r="G3">
-        <v>41</v>
-      </c>
-      <c r="H3">
-        <v>45</v>
-      </c>
       <c r="I3">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="J3">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="K3">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L3">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M3">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="N3">
         <v>55</v>
@@ -640,52 +640,52 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="H4">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I4">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J4">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="K4">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="L4">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="M4">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="N4">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="O4">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="P4">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="Q4">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -693,40 +693,40 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>7</v>
       </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="F5">
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="G5">
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>11</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
         <v>12</v>
-      </c>
-      <c r="K5">
-        <v>12</v>
-      </c>
-      <c r="L5">
-        <v>13</v>
-      </c>
-      <c r="M5">
-        <v>15</v>
       </c>
       <c r="N5">
         <v>15</v>
@@ -746,52 +746,52 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J6">
+        <v>36</v>
+      </c>
+      <c r="K6">
+        <v>42</v>
+      </c>
+      <c r="L6">
         <v>45</v>
       </c>
-      <c r="K6">
-        <v>51</v>
-      </c>
-      <c r="L6">
+      <c r="M6">
+        <v>46</v>
+      </c>
+      <c r="N6">
+        <v>52</v>
+      </c>
+      <c r="O6">
+        <v>52</v>
+      </c>
+      <c r="P6">
         <v>54</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <v>55</v>
-      </c>
-      <c r="N6">
-        <v>56</v>
-      </c>
-      <c r="O6">
-        <v>56</v>
-      </c>
-      <c r="P6">
-        <v>58</v>
-      </c>
-      <c r="Q6">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -799,52 +799,52 @@
         <v>21</v>
       </c>
       <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
       <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
         <v>11</v>
       </c>
-      <c r="F7">
+      <c r="K7">
         <v>12</v>
       </c>
-      <c r="G7">
+      <c r="L7">
         <v>12</v>
       </c>
-      <c r="H7">
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7">
         <v>14</v>
       </c>
-      <c r="I7">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>15</v>
-      </c>
-      <c r="K7">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>16</v>
-      </c>
-      <c r="N7">
-        <v>16</v>
-      </c>
       <c r="O7">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P7">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="Q7">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -852,52 +852,52 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>9</v>
+      </c>
+      <c r="L8">
         <v>11</v>
       </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>14</v>
-      </c>
-      <c r="J8">
-        <v>14</v>
-      </c>
-      <c r="K8">
-        <v>14</v>
-      </c>
-      <c r="L8">
+      <c r="M8">
+        <v>13</v>
+      </c>
+      <c r="N8">
+        <v>15</v>
+      </c>
+      <c r="O8">
         <v>16</v>
       </c>
-      <c r="M8">
-        <v>17</v>
-      </c>
-      <c r="N8">
-        <v>17</v>
-      </c>
-      <c r="O8">
+      <c r="P8">
+        <v>15</v>
+      </c>
+      <c r="Q8">
         <v>18</v>
-      </c>
-      <c r="P8">
-        <v>17</v>
-      </c>
-      <c r="Q8">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -905,52 +905,52 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
         <v>21</v>
       </c>
-      <c r="E9">
-        <v>34</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
       <c r="G9">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H9">
+        <v>23</v>
+      </c>
+      <c r="I9">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <v>28</v>
+      </c>
+      <c r="K9">
+        <v>28</v>
+      </c>
+      <c r="L9">
+        <v>28</v>
+      </c>
+      <c r="M9">
+        <v>29</v>
+      </c>
+      <c r="N9">
+        <v>31</v>
+      </c>
+      <c r="O9">
         <v>32</v>
       </c>
-      <c r="I9">
-        <v>37</v>
-      </c>
-      <c r="J9">
-        <v>38</v>
-      </c>
-      <c r="K9">
-        <v>38</v>
-      </c>
-      <c r="L9">
-        <v>37</v>
-      </c>
-      <c r="M9">
-        <v>38</v>
-      </c>
-      <c r="N9">
-        <v>38</v>
-      </c>
-      <c r="O9">
-        <v>39</v>
-      </c>
       <c r="P9">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q9">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -976,34 +976,34 @@
         <v>0</v>
       </c>
       <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
         <v>13</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>13</v>
       </c>
-      <c r="J10">
-        <v>12</v>
-      </c>
-      <c r="K10">
-        <v>12</v>
-      </c>
-      <c r="L10">
-        <v>12</v>
-      </c>
-      <c r="M10">
-        <v>12</v>
-      </c>
-      <c r="N10">
-        <v>14</v>
-      </c>
-      <c r="O10">
-        <v>14</v>
-      </c>
       <c r="P10">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q10">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1011,52 +1011,52 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>105</v>
+        <v>43</v>
       </c>
       <c r="C11">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="D11">
-        <v>212</v>
+        <v>80</v>
       </c>
       <c r="E11">
-        <v>254</v>
+        <v>111</v>
       </c>
       <c r="F11">
-        <v>289</v>
+        <v>134</v>
       </c>
       <c r="G11">
-        <v>301</v>
+        <v>141</v>
       </c>
       <c r="H11">
-        <v>318</v>
+        <v>148</v>
       </c>
       <c r="I11">
-        <v>324</v>
+        <v>155</v>
       </c>
       <c r="J11">
-        <v>341</v>
+        <v>172</v>
       </c>
       <c r="K11">
-        <v>338</v>
+        <v>165</v>
       </c>
       <c r="L11">
-        <v>359</v>
+        <v>187</v>
       </c>
       <c r="M11">
-        <v>363</v>
+        <v>192</v>
       </c>
       <c r="N11">
-        <v>380</v>
+        <v>242</v>
       </c>
       <c r="O11">
-        <v>384</v>
+        <v>250</v>
       </c>
       <c r="P11">
-        <v>377</v>
+        <v>251</v>
       </c>
       <c r="Q11">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1064,52 +1064,52 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C12">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="D12">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="E12">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="F12">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="G12">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="H12">
+        <v>43</v>
+      </c>
+      <c r="I12">
+        <v>45</v>
+      </c>
+      <c r="J12">
+        <v>52</v>
+      </c>
+      <c r="K12">
+        <v>56</v>
+      </c>
+      <c r="L12">
+        <v>62</v>
+      </c>
+      <c r="M12">
+        <v>70</v>
+      </c>
+      <c r="N12">
+        <v>87</v>
+      </c>
+      <c r="O12">
+        <v>90</v>
+      </c>
+      <c r="P12">
         <v>92</v>
       </c>
-      <c r="I12">
+      <c r="Q12">
         <v>93</v>
-      </c>
-      <c r="J12">
-        <v>100</v>
-      </c>
-      <c r="K12">
-        <v>104</v>
-      </c>
-      <c r="L12">
-        <v>108</v>
-      </c>
-      <c r="M12">
-        <v>117</v>
-      </c>
-      <c r="N12">
-        <v>119</v>
-      </c>
-      <c r="O12">
-        <v>120</v>
-      </c>
-      <c r="P12">
-        <v>122</v>
-      </c>
-      <c r="Q12">
-        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1117,52 +1117,52 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E13">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="F13">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="G13">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="H13">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="I13">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="J13">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="K13">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="L13">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="M13">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="N13">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="O13">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="P13">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="Q13">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1170,52 +1170,52 @@
         <v>28</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="G14">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="H14">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="I14">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="J14">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="K14">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="L14">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="M14">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="N14">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="O14">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="P14">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="Q14">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1223,52 +1223,52 @@
         <v>29</v>
       </c>
       <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
         <v>25</v>
       </c>
-      <c r="C15">
-        <v>28</v>
-      </c>
-      <c r="D15">
+      <c r="F15">
+        <v>29</v>
+      </c>
+      <c r="G15">
+        <v>31</v>
+      </c>
+      <c r="H15">
+        <v>34</v>
+      </c>
+      <c r="I15">
+        <v>35</v>
+      </c>
+      <c r="J15">
         <v>42</v>
       </c>
-      <c r="E15">
-        <v>50</v>
-      </c>
-      <c r="F15">
+      <c r="K15">
+        <v>43</v>
+      </c>
+      <c r="L15">
+        <v>44</v>
+      </c>
+      <c r="M15">
+        <v>45</v>
+      </c>
+      <c r="N15">
         <v>57</v>
       </c>
-      <c r="G15">
-        <v>59</v>
-      </c>
-      <c r="H15">
-        <v>62</v>
-      </c>
-      <c r="I15">
-        <v>63</v>
-      </c>
-      <c r="J15">
-        <v>71</v>
-      </c>
-      <c r="K15">
-        <v>71</v>
-      </c>
-      <c r="L15">
-        <v>72</v>
-      </c>
-      <c r="M15">
-        <v>73</v>
-      </c>
-      <c r="N15">
-        <v>76</v>
-      </c>
       <c r="O15">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="P15">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="Q15">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1276,52 +1276,52 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C16">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D16">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="F16">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="G16">
-        <v>97</v>
+        <v>43</v>
       </c>
       <c r="H16">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="I16">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="J16">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="K16">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="L16">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="M16">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="N16">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="O16">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="P16">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="Q16">
-        <v>112</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1329,52 +1329,52 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>39180</v>
+        <v>39</v>
       </c>
       <c r="D17">
-        <v>74</v>
+        <v>17</v>
       </c>
       <c r="E17">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="G17">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="H17">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="I17">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="J17">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="K17">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="L17">
-        <v>130</v>
+        <v>47</v>
       </c>
       <c r="M17">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="N17">
-        <v>132</v>
+        <v>73</v>
       </c>
       <c r="O17">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="P17">
-        <v>134</v>
+        <v>75</v>
       </c>
       <c r="Q17">
-        <v>140</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1382,52 +1382,52 @@
         <v>32</v>
       </c>
       <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+      <c r="D18">
+        <v>33</v>
+      </c>
+      <c r="E18">
+        <v>55</v>
+      </c>
+      <c r="F18">
         <v>62</v>
       </c>
-      <c r="C18">
-        <v>67</v>
-      </c>
-      <c r="D18">
-        <v>85</v>
-      </c>
-      <c r="E18">
-        <v>113</v>
-      </c>
-      <c r="F18">
-        <v>114</v>
-      </c>
       <c r="G18">
-        <v>124</v>
+        <v>71</v>
       </c>
       <c r="H18">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="I18">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="J18">
-        <v>144</v>
+        <v>87</v>
       </c>
       <c r="K18">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="L18">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="M18">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="N18">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="O18">
-        <v>171</v>
+        <v>130</v>
       </c>
       <c r="P18">
-        <v>176</v>
+        <v>135</v>
       </c>
       <c r="Q18">
-        <v>182</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1435,52 +1435,52 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D19">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E19">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G19">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H19">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I19">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="J19">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="K19">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="L19">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="M19">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="N19">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="O19">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="P19">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q19">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>